<commit_message>
Ticket writer now properly assigns input values to selected cells/rows
</commit_message>
<xml_diff>
--- a/src/main/resources/demoTicket.xlsx
+++ b/src/main/resources/demoTicket.xlsx
@@ -12,30 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Head First Java</t>
+    <t>name</t>
   </si>
   <si>
-    <t>Kathy Serria</t>
-  </si>
-  <si>
-    <t>Effective Java</t>
-  </si>
-  <si>
-    <t>Joshua Bloch</t>
-  </si>
-  <si>
-    <t>Clean Code</t>
-  </si>
-  <si>
-    <t>Robert martin</t>
-  </si>
-  <si>
-    <t>Thinking in Java</t>
-  </si>
-  <si>
-    <t>Bruce Eckel</t>
+    <t>surename</t>
   </si>
 </sst>
 </file>
@@ -86,48 +68,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="2">
-      <c r="B2" t="s">
+    <row r="3">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="n">
-        <v>79.0</v>
+      <c r="H3" t="n">
+        <v>69.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="B3" t="s">
-        <v>2</v>
+    <row r="8">
+      <c r="C8" t="n">
+        <v>7331.0</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>35.0</v>
+      <c r="D8" t="n">
+        <v>1337.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
connected TicketWriter to corresponding array lists (lots of bugs)
</commit_message>
<xml_diff>
--- a/src/main/resources/demoTicket.xlsx
+++ b/src/main/resources/demoTicket.xlsx
@@ -12,14 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>surename</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -69,22 +62,18 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="3">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3"/>
       <c r="H3" t="n">
-        <v>69.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" t="n">
-        <v>7331.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n">
-        <v>1337.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/eenobai/BookingService"
This reverts commit 313c32f8a3b9c56a0b16279f45e21884ba4346fb, reversing
changes made to 859357638cbffb1c924091bbca71863d630eb013.
</commit_message>
<xml_diff>
--- a/src/main/resources/demoTicket.xlsx
+++ b/src/main/resources/demoTicket.xlsx
@@ -12,7 +12,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Head First Java</t>
+  </si>
+  <si>
+    <t>Kathy Serria</t>
+  </si>
+  <si>
+    <t>Effective Java</t>
+  </si>
+  <si>
+    <t>Joshua Bloch</t>
+  </si>
+  <si>
+    <t>Clean Code</t>
+  </si>
+  <si>
+    <t>Robert martin</t>
+  </si>
+  <si>
+    <t>Thinking in Java</t>
+  </si>
+  <si>
+    <t>Bruce Eckel</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -61,19 +86,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="3">
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="H3" t="n">
-        <v>0.0</v>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>79.0</v>
       </c>
     </row>
-    <row r="8">
-      <c r="C8" t="n">
-        <v>0.0</v>
+    <row r="3">
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
-      <c r="D8" t="n">
-        <v>0.0</v>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="n">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="n">
+        <v>42.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="n">
+        <v>35.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fully working comparing tool
</commit_message>
<xml_diff>
--- a/src/main/resources/demoTicket.xlsx
+++ b/src/main/resources/demoTicket.xlsx
@@ -20,10 +20,10 @@
     <t>w</t>
   </si>
   <si>
-    <t>location 9</t>
+    <t>location 4</t>
   </si>
   <si>
-    <t>name 9</t>
+    <t>name 4</t>
   </si>
 </sst>
 </file>

</xml_diff>